<commit_message>
NOK Details pulling through on upgrades
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/PrintTemplateUpgrade3Transfer.xlsx
+++ b/UDM.Insurance.Interface/Templates/PrintTemplateUpgrade3Transfer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyleh\source\repos\Insure20230223\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FDD0E0-9525-4299-A38D-02D5F5275D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82298F90-110D-4074-98C8-FF62234F0266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3345" windowWidth="24240" windowHeight="13020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -52,6 +52,7 @@
     <definedName name="LifeAssured2FirstName" localSheetId="4">'Cover And Lead'!$AX$46</definedName>
     <definedName name="LifeAssured2Surname">'Cover And Lead'!$AX$47</definedName>
     <definedName name="NewTotalPremium" localSheetId="4">'Cover And Lead'!$AJ$48</definedName>
+    <definedName name="NOKDetails">'Cover And Lead'!$AJ$50</definedName>
     <definedName name="Offer">'Cover And Lead'!$V$48</definedName>
     <definedName name="PostalCode" localSheetId="4">'Cover And Lead'!$AP$42</definedName>
     <definedName name="RefNo" localSheetId="4">'Cover And Lead'!$A$42</definedName>
@@ -804,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1212,6 +1213,33 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1239,33 +1267,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1292,6 +1293,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1509,9 +1513,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1549,9 +1553,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1584,26 +1588,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1636,26 +1623,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1835,17 +1805,17 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
-    <col min="2" max="3" width="24.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="51" t="s">
         <v>14</v>
       </c>
@@ -1854,7 +1824,7 @@
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1871,126 +1841,126 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2015,13 +1985,13 @@
       <selection activeCell="F5" sqref="F5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="75" width="2.54296875" style="15" customWidth="1"/>
-    <col min="76" max="16384" width="9.1796875" style="15"/>
+    <col min="1" max="75" width="2.5703125" style="15" customWidth="1"/>
+    <col min="76" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="52" t="s">
         <v>34</v>
       </c>
@@ -2098,7 +2068,7 @@
       <c r="BB1" s="52"/>
       <c r="BC1" s="52"/>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2" s="71"/>
       <c r="B2" s="71"/>
       <c r="C2" s="71"/>
@@ -2155,7 +2125,7 @@
       <c r="BB2" s="63"/>
       <c r="BC2" s="63"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" s="71"/>
       <c r="B3" s="71"/>
       <c r="C3" s="71"/>
@@ -2212,7 +2182,7 @@
       <c r="BB3" s="63"/>
       <c r="BC3" s="63"/>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" s="52" t="s">
         <v>64</v>
       </c>
@@ -2287,7 +2257,7 @@
       <c r="BB4" s="52"/>
       <c r="BC4" s="52"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A5" s="53"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -2344,7 +2314,7 @@
       <c r="BB5" s="64"/>
       <c r="BC5" s="64"/>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A6" s="52" t="s">
         <v>44</v>
       </c>
@@ -2418,7 +2388,7 @@
       <c r="BC6" s="52"/>
       <c r="BD6" s="17"/>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" s="53"/>
       <c r="B7" s="53"/>
       <c r="C7" s="53"/>
@@ -2476,7 +2446,7 @@
       <c r="BC7" s="53"/>
       <c r="BD7" s="16"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" s="52" t="s">
         <v>63</v>
       </c>
@@ -2543,7 +2513,7 @@
       <c r="BB8" s="52"/>
       <c r="BC8" s="52"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A9" s="61"/>
       <c r="B9" s="61"/>
       <c r="C9" s="61"/>
@@ -2600,7 +2570,7 @@
       <c r="BB9" s="60"/>
       <c r="BC9" s="60"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
         <v>54</v>
       </c>
@@ -2673,7 +2643,7 @@
       <c r="BB10" s="62"/>
       <c r="BC10" s="62"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A11" s="57"/>
       <c r="B11" s="58"/>
       <c r="C11" s="58"/>
@@ -2730,7 +2700,7 @@
       <c r="BB11" s="62"/>
       <c r="BC11" s="62"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>55</v>
       </c>
@@ -2789,7 +2759,7 @@
       <c r="BB12" s="62"/>
       <c r="BC12" s="62"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A13" s="57"/>
       <c r="B13" s="58"/>
       <c r="C13" s="58"/>
@@ -2935,12 +2905,12 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="55" width="2.54296875" customWidth="1"/>
+    <col min="1" max="55" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -2997,8 +2967,8 @@
       <c r="BB1" s="15"/>
       <c r="BC1" s="15"/>
     </row>
-    <row r="2" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -3051,54 +3021,54 @@
       <c r="AZ3" s="8"/>
       <c r="BA3" s="9"/>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C4" s="10"/>
       <c r="BA4" s="11"/>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="BA5" s="11"/>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C6" s="10"/>
       <c r="BA6" s="11"/>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C7" s="10"/>
       <c r="BA7" s="11"/>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C8" s="10"/>
       <c r="BA8" s="11"/>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C9" s="10"/>
       <c r="BA9" s="11"/>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C10" s="10"/>
       <c r="BA10" s="11"/>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C11" s="10"/>
       <c r="BA11" s="11"/>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C12" s="10"/>
       <c r="BA12" s="11"/>
     </row>
-    <row r="13" spans="1:55" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:55" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C13" s="10"/>
       <c r="W13" s="50" t="s">
         <v>85</v>
       </c>
       <c r="BA13" s="11"/>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
       <c r="BA14" s="11"/>
     </row>
-    <row r="15" spans="1:55" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:55" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C15" s="19"/>
       <c r="P15" s="73" t="s">
         <v>0</v>
@@ -3141,7 +3111,7 @@
       <c r="AZ15" s="76"/>
       <c r="BA15" s="20"/>
     </row>
-    <row r="16" spans="1:55" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:55" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C16" s="19"/>
       <c r="P16" s="73" t="s">
         <v>1</v>
@@ -3184,7 +3154,7 @@
       <c r="AZ16" s="76"/>
       <c r="BA16" s="20"/>
     </row>
-    <row r="17" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C17" s="19"/>
       <c r="P17" s="73" t="s">
         <v>2</v>
@@ -3227,7 +3197,7 @@
       <c r="AZ17" s="76"/>
       <c r="BA17" s="20"/>
     </row>
-    <row r="18" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C18" s="19"/>
       <c r="P18" s="73" t="s">
         <v>3</v>
@@ -3270,7 +3240,7 @@
       <c r="AZ18" s="76"/>
       <c r="BA18" s="20"/>
     </row>
-    <row r="19" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C19" s="19"/>
       <c r="P19" s="73" t="s">
         <v>4</v>
@@ -3313,7 +3283,7 @@
       <c r="AZ19" s="77"/>
       <c r="BA19" s="20"/>
     </row>
-    <row r="20" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C20" s="19"/>
       <c r="P20" s="73" t="s">
         <v>66</v>
@@ -3356,7 +3326,7 @@
       <c r="AZ20" s="74"/>
       <c r="BA20" s="20"/>
     </row>
-    <row r="21" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C21" s="19"/>
       <c r="P21" s="73" t="s">
         <v>5</v>
@@ -3399,11 +3369,11 @@
       <c r="AZ21" s="74"/>
       <c r="BA21" s="20"/>
     </row>
-    <row r="22" spans="3:53" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
       <c r="BA22" s="11"/>
     </row>
-    <row r="23" spans="3:53" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:53" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="10"/>
       <c r="P23" s="75" t="s">
         <v>86</v>
@@ -3446,7 +3416,7 @@
       <c r="AZ23" s="75"/>
       <c r="BA23" s="11"/>
     </row>
-    <row r="24" spans="3:53" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:53" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="10"/>
       <c r="P24" s="75"/>
       <c r="Q24" s="75"/>
@@ -3487,15 +3457,15 @@
       <c r="AZ24" s="75"/>
       <c r="BA24" s="11"/>
     </row>
-    <row r="25" spans="3:53" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C25" s="10"/>
       <c r="BA25" s="11"/>
     </row>
-    <row r="26" spans="3:53" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C26" s="10"/>
       <c r="BA26" s="11"/>
     </row>
-    <row r="27" spans="3:53" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="12"/>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
@@ -3580,12 +3550,12 @@
       <selection activeCell="B30" sqref="B30:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="110" t="s">
         <v>0</v>
       </c>
@@ -3597,7 +3567,7 @@
       <c r="H2" s="115"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:11" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="116" t="s">
         <v>15</v>
       </c>
@@ -3609,10 +3579,10 @@
       <c r="H3" s="121"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="95" t="s">
         <v>16</v>
       </c>
@@ -3623,7 +3593,7 @@
       <c r="G6" s="108"/>
       <c r="H6" s="109"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="95" t="s">
         <v>17</v>
       </c>
@@ -3634,7 +3604,7 @@
       <c r="G7" s="108"/>
       <c r="H7" s="109"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="95" t="s">
         <v>18</v>
       </c>
@@ -3645,7 +3615,7 @@
       <c r="G8" s="108"/>
       <c r="H8" s="109"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="95" t="s">
         <v>19</v>
       </c>
@@ -3656,7 +3626,7 @@
       <c r="G9" s="108"/>
       <c r="H9" s="109"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="95" t="s">
         <v>20</v>
       </c>
@@ -3667,7 +3637,7 @@
       <c r="G10" s="99"/>
       <c r="H10" s="100"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="95" t="s">
         <v>21</v>
       </c>
@@ -3680,7 +3650,7 @@
       <c r="G13" s="96"/>
       <c r="H13" s="97"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="101"/>
       <c r="C14" s="102"/>
       <c r="D14" s="103"/>
@@ -3689,7 +3659,7 @@
       <c r="G14" s="105"/>
       <c r="H14" s="106"/>
     </row>
-    <row r="16" spans="2:11" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="92" t="s">
         <v>22</v>
       </c>
@@ -3703,7 +3673,7 @@
       <c r="J16" s="93"/>
       <c r="K16" s="94"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -3715,7 +3685,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -3727,7 +3697,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -3739,7 +3709,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -3751,7 +3721,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3763,7 +3733,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="92" t="s">
         <v>23</v>
       </c>
@@ -3777,7 +3747,7 @@
       <c r="J22" s="93"/>
       <c r="K22" s="94"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3789,7 +3759,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="25" spans="2:14" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="92" t="s">
         <v>24</v>
       </c>
@@ -3816,7 +3786,7 @@
       </c>
       <c r="N25" s="91"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="85" t="s">
         <v>29</v>
       </c>
@@ -3833,7 +3803,7 @@
       <c r="M26" s="88"/>
       <c r="N26" s="89"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="79" t="s">
         <v>30</v>
       </c>
@@ -3850,7 +3820,7 @@
       <c r="M27" s="83"/>
       <c r="N27" s="84"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="85" t="s">
         <v>31</v>
       </c>
@@ -3867,7 +3837,7 @@
       <c r="M28" s="78"/>
       <c r="N28" s="78"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="79" t="s">
         <v>32</v>
       </c>
@@ -3884,7 +3854,7 @@
       <c r="M29" s="82"/>
       <c r="N29" s="82"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="85" t="s">
         <v>33</v>
       </c>
@@ -3969,19 +3939,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BD306"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A11" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A20" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="AJ50" sqref="AJ50:AP55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="1.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="1.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="55" width="2.453125" customWidth="1"/>
-    <col min="56" max="61" width="1.1796875" customWidth="1"/>
+    <col min="1" max="55" width="2.42578125" customWidth="1"/>
+    <col min="56" max="61" width="1.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:53" s="15" customFormat="1" ht="12.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="3:53" s="15" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C3" s="21"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -4034,63 +4004,63 @@
       <c r="AZ3" s="22"/>
       <c r="BA3" s="23"/>
     </row>
-    <row r="4" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C4" s="24"/>
       <c r="BA4" s="25"/>
     </row>
-    <row r="5" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C5" s="24"/>
       <c r="BA5" s="25"/>
     </row>
-    <row r="6" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C6" s="24"/>
       <c r="BA6" s="25"/>
     </row>
-    <row r="7" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C7" s="24"/>
       <c r="BA7" s="25"/>
     </row>
-    <row r="8" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C8" s="24"/>
       <c r="BA8" s="25"/>
     </row>
-    <row r="9" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C9" s="24"/>
       <c r="BA9" s="25"/>
     </row>
-    <row r="10" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C10" s="24"/>
       <c r="BA10" s="25"/>
     </row>
-    <row r="11" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C11" s="24"/>
       <c r="BA11" s="25"/>
     </row>
-    <row r="12" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C12" s="24"/>
       <c r="BA12" s="25"/>
     </row>
-    <row r="13" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C13" s="24"/>
       <c r="BA13" s="25"/>
     </row>
-    <row r="14" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C14" s="24"/>
       <c r="BA14" s="25"/>
     </row>
-    <row r="15" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C15" s="24"/>
       <c r="BA15" s="25"/>
     </row>
-    <row r="16" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C16" s="24"/>
       <c r="BA16" s="25"/>
     </row>
-    <row r="17" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C17" s="24"/>
       <c r="BA17" s="25"/>
     </row>
-    <row r="18" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C18" s="19"/>
       <c r="P18" s="73" t="s">
         <v>0</v>
@@ -4133,7 +4103,7 @@
       <c r="AZ18" s="76"/>
       <c r="BA18" s="20"/>
     </row>
-    <row r="19" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C19" s="19"/>
       <c r="P19" s="73" t="s">
         <v>1</v>
@@ -4176,7 +4146,7 @@
       <c r="AZ19" s="76"/>
       <c r="BA19" s="20"/>
     </row>
-    <row r="20" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C20" s="19"/>
       <c r="P20" s="73" t="s">
         <v>2</v>
@@ -4219,7 +4189,7 @@
       <c r="AZ20" s="76"/>
       <c r="BA20" s="20"/>
     </row>
-    <row r="21" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C21" s="19"/>
       <c r="P21" s="73" t="s">
         <v>3</v>
@@ -4262,7 +4232,7 @@
       <c r="AZ21" s="76"/>
       <c r="BA21" s="20"/>
     </row>
-    <row r="22" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C22" s="19"/>
       <c r="P22" s="73" t="s">
         <v>4</v>
@@ -4305,7 +4275,7 @@
       <c r="AZ22" s="76"/>
       <c r="BA22" s="20"/>
     </row>
-    <row r="23" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C23" s="19"/>
       <c r="P23" s="73" t="s">
         <v>66</v>
@@ -4348,7 +4318,7 @@
       <c r="AZ23" s="74"/>
       <c r="BA23" s="20"/>
     </row>
-    <row r="24" spans="3:53" s="18" customFormat="1" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="3:53" s="18" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C24" s="19"/>
       <c r="P24" s="73" t="s">
         <v>5</v>
@@ -4391,189 +4361,189 @@
       <c r="AZ24" s="74"/>
       <c r="BA24" s="20"/>
     </row>
-    <row r="25" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C25" s="24"/>
       <c r="BA25" s="25"/>
     </row>
-    <row r="26" spans="3:53" s="15" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:53" s="15" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="24"/>
-      <c r="P26" s="168" t="s">
+      <c r="P26" s="157" t="s">
         <v>85</v>
       </c>
-      <c r="Q26" s="169"/>
-      <c r="R26" s="169"/>
-      <c r="S26" s="169"/>
-      <c r="T26" s="169"/>
-      <c r="U26" s="169"/>
-      <c r="V26" s="169"/>
-      <c r="W26" s="169"/>
-      <c r="X26" s="169"/>
-      <c r="Y26" s="169"/>
-      <c r="Z26" s="169"/>
-      <c r="AA26" s="169"/>
-      <c r="AB26" s="169"/>
-      <c r="AC26" s="169"/>
-      <c r="AD26" s="169"/>
-      <c r="AE26" s="169"/>
-      <c r="AF26" s="169"/>
-      <c r="AG26" s="169"/>
-      <c r="AH26" s="169"/>
-      <c r="AI26" s="169"/>
-      <c r="AJ26" s="169"/>
-      <c r="AK26" s="169"/>
-      <c r="AL26" s="169"/>
-      <c r="AM26" s="169"/>
-      <c r="AN26" s="169"/>
-      <c r="AO26" s="169"/>
-      <c r="AP26" s="169"/>
-      <c r="AQ26" s="169"/>
-      <c r="AR26" s="169"/>
-      <c r="AS26" s="169"/>
-      <c r="AT26" s="169"/>
-      <c r="AU26" s="169"/>
-      <c r="AV26" s="169"/>
-      <c r="AW26" s="169"/>
-      <c r="AX26" s="169"/>
-      <c r="AY26" s="169"/>
-      <c r="AZ26" s="170"/>
+      <c r="Q26" s="158"/>
+      <c r="R26" s="158"/>
+      <c r="S26" s="158"/>
+      <c r="T26" s="158"/>
+      <c r="U26" s="158"/>
+      <c r="V26" s="158"/>
+      <c r="W26" s="158"/>
+      <c r="X26" s="158"/>
+      <c r="Y26" s="158"/>
+      <c r="Z26" s="158"/>
+      <c r="AA26" s="158"/>
+      <c r="AB26" s="158"/>
+      <c r="AC26" s="158"/>
+      <c r="AD26" s="158"/>
+      <c r="AE26" s="158"/>
+      <c r="AF26" s="158"/>
+      <c r="AG26" s="158"/>
+      <c r="AH26" s="158"/>
+      <c r="AI26" s="158"/>
+      <c r="AJ26" s="158"/>
+      <c r="AK26" s="158"/>
+      <c r="AL26" s="158"/>
+      <c r="AM26" s="158"/>
+      <c r="AN26" s="158"/>
+      <c r="AO26" s="158"/>
+      <c r="AP26" s="158"/>
+      <c r="AQ26" s="158"/>
+      <c r="AR26" s="158"/>
+      <c r="AS26" s="158"/>
+      <c r="AT26" s="158"/>
+      <c r="AU26" s="158"/>
+      <c r="AV26" s="158"/>
+      <c r="AW26" s="158"/>
+      <c r="AX26" s="158"/>
+      <c r="AY26" s="158"/>
+      <c r="AZ26" s="159"/>
       <c r="BA26" s="25"/>
     </row>
-    <row r="27" spans="3:53" s="15" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:53" s="15" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="24"/>
-      <c r="P27" s="171"/>
-      <c r="Q27" s="172"/>
-      <c r="R27" s="172"/>
-      <c r="S27" s="172"/>
-      <c r="T27" s="172"/>
-      <c r="U27" s="172"/>
-      <c r="V27" s="172"/>
-      <c r="W27" s="172"/>
-      <c r="X27" s="172"/>
-      <c r="Y27" s="172"/>
-      <c r="Z27" s="172"/>
-      <c r="AA27" s="172"/>
-      <c r="AB27" s="172"/>
-      <c r="AC27" s="172"/>
-      <c r="AD27" s="172"/>
-      <c r="AE27" s="172"/>
-      <c r="AF27" s="172"/>
-      <c r="AG27" s="172"/>
-      <c r="AH27" s="172"/>
-      <c r="AI27" s="172"/>
-      <c r="AJ27" s="172"/>
-      <c r="AK27" s="172"/>
-      <c r="AL27" s="172"/>
-      <c r="AM27" s="172"/>
-      <c r="AN27" s="172"/>
-      <c r="AO27" s="172"/>
-      <c r="AP27" s="172"/>
-      <c r="AQ27" s="172"/>
-      <c r="AR27" s="172"/>
-      <c r="AS27" s="172"/>
-      <c r="AT27" s="172"/>
-      <c r="AU27" s="172"/>
-      <c r="AV27" s="172"/>
-      <c r="AW27" s="172"/>
-      <c r="AX27" s="172"/>
-      <c r="AY27" s="172"/>
-      <c r="AZ27" s="173"/>
+      <c r="P27" s="160"/>
+      <c r="Q27" s="161"/>
+      <c r="R27" s="161"/>
+      <c r="S27" s="161"/>
+      <c r="T27" s="161"/>
+      <c r="U27" s="161"/>
+      <c r="V27" s="161"/>
+      <c r="W27" s="161"/>
+      <c r="X27" s="161"/>
+      <c r="Y27" s="161"/>
+      <c r="Z27" s="161"/>
+      <c r="AA27" s="161"/>
+      <c r="AB27" s="161"/>
+      <c r="AC27" s="161"/>
+      <c r="AD27" s="161"/>
+      <c r="AE27" s="161"/>
+      <c r="AF27" s="161"/>
+      <c r="AG27" s="161"/>
+      <c r="AH27" s="161"/>
+      <c r="AI27" s="161"/>
+      <c r="AJ27" s="161"/>
+      <c r="AK27" s="161"/>
+      <c r="AL27" s="161"/>
+      <c r="AM27" s="161"/>
+      <c r="AN27" s="161"/>
+      <c r="AO27" s="161"/>
+      <c r="AP27" s="161"/>
+      <c r="AQ27" s="161"/>
+      <c r="AR27" s="161"/>
+      <c r="AS27" s="161"/>
+      <c r="AT27" s="161"/>
+      <c r="AU27" s="161"/>
+      <c r="AV27" s="161"/>
+      <c r="AW27" s="161"/>
+      <c r="AX27" s="161"/>
+      <c r="AY27" s="161"/>
+      <c r="AZ27" s="162"/>
       <c r="BA27" s="25"/>
     </row>
-    <row r="28" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C28" s="24"/>
-      <c r="P28" s="171"/>
-      <c r="Q28" s="172"/>
-      <c r="R28" s="172"/>
-      <c r="S28" s="172"/>
-      <c r="T28" s="172"/>
-      <c r="U28" s="172"/>
-      <c r="V28" s="172"/>
-      <c r="W28" s="172"/>
-      <c r="X28" s="172"/>
-      <c r="Y28" s="172"/>
-      <c r="Z28" s="172"/>
-      <c r="AA28" s="172"/>
-      <c r="AB28" s="172"/>
-      <c r="AC28" s="172"/>
-      <c r="AD28" s="172"/>
-      <c r="AE28" s="172"/>
-      <c r="AF28" s="172"/>
-      <c r="AG28" s="172"/>
-      <c r="AH28" s="172"/>
-      <c r="AI28" s="172"/>
-      <c r="AJ28" s="172"/>
-      <c r="AK28" s="172"/>
-      <c r="AL28" s="172"/>
-      <c r="AM28" s="172"/>
-      <c r="AN28" s="172"/>
-      <c r="AO28" s="172"/>
-      <c r="AP28" s="172"/>
-      <c r="AQ28" s="172"/>
-      <c r="AR28" s="172"/>
-      <c r="AS28" s="172"/>
-      <c r="AT28" s="172"/>
-      <c r="AU28" s="172"/>
-      <c r="AV28" s="172"/>
-      <c r="AW28" s="172"/>
-      <c r="AX28" s="172"/>
-      <c r="AY28" s="172"/>
-      <c r="AZ28" s="173"/>
+      <c r="P28" s="160"/>
+      <c r="Q28" s="161"/>
+      <c r="R28" s="161"/>
+      <c r="S28" s="161"/>
+      <c r="T28" s="161"/>
+      <c r="U28" s="161"/>
+      <c r="V28" s="161"/>
+      <c r="W28" s="161"/>
+      <c r="X28" s="161"/>
+      <c r="Y28" s="161"/>
+      <c r="Z28" s="161"/>
+      <c r="AA28" s="161"/>
+      <c r="AB28" s="161"/>
+      <c r="AC28" s="161"/>
+      <c r="AD28" s="161"/>
+      <c r="AE28" s="161"/>
+      <c r="AF28" s="161"/>
+      <c r="AG28" s="161"/>
+      <c r="AH28" s="161"/>
+      <c r="AI28" s="161"/>
+      <c r="AJ28" s="161"/>
+      <c r="AK28" s="161"/>
+      <c r="AL28" s="161"/>
+      <c r="AM28" s="161"/>
+      <c r="AN28" s="161"/>
+      <c r="AO28" s="161"/>
+      <c r="AP28" s="161"/>
+      <c r="AQ28" s="161"/>
+      <c r="AR28" s="161"/>
+      <c r="AS28" s="161"/>
+      <c r="AT28" s="161"/>
+      <c r="AU28" s="161"/>
+      <c r="AV28" s="161"/>
+      <c r="AW28" s="161"/>
+      <c r="AX28" s="161"/>
+      <c r="AY28" s="161"/>
+      <c r="AZ28" s="162"/>
       <c r="BA28" s="25"/>
     </row>
-    <row r="29" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C29" s="24"/>
-      <c r="P29" s="174"/>
-      <c r="Q29" s="175"/>
-      <c r="R29" s="175"/>
-      <c r="S29" s="175"/>
-      <c r="T29" s="175"/>
-      <c r="U29" s="175"/>
-      <c r="V29" s="175"/>
-      <c r="W29" s="175"/>
-      <c r="X29" s="175"/>
-      <c r="Y29" s="175"/>
-      <c r="Z29" s="175"/>
-      <c r="AA29" s="175"/>
-      <c r="AB29" s="175"/>
-      <c r="AC29" s="175"/>
-      <c r="AD29" s="175"/>
-      <c r="AE29" s="175"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="175"/>
-      <c r="AH29" s="175"/>
-      <c r="AI29" s="175"/>
-      <c r="AJ29" s="175"/>
-      <c r="AK29" s="175"/>
-      <c r="AL29" s="175"/>
-      <c r="AM29" s="175"/>
-      <c r="AN29" s="175"/>
-      <c r="AO29" s="175"/>
-      <c r="AP29" s="175"/>
-      <c r="AQ29" s="175"/>
-      <c r="AR29" s="175"/>
-      <c r="AS29" s="175"/>
-      <c r="AT29" s="175"/>
-      <c r="AU29" s="175"/>
-      <c r="AV29" s="175"/>
-      <c r="AW29" s="175"/>
-      <c r="AX29" s="175"/>
-      <c r="AY29" s="175"/>
-      <c r="AZ29" s="176"/>
+      <c r="P29" s="163"/>
+      <c r="Q29" s="164"/>
+      <c r="R29" s="164"/>
+      <c r="S29" s="164"/>
+      <c r="T29" s="164"/>
+      <c r="U29" s="164"/>
+      <c r="V29" s="164"/>
+      <c r="W29" s="164"/>
+      <c r="X29" s="164"/>
+      <c r="Y29" s="164"/>
+      <c r="Z29" s="164"/>
+      <c r="AA29" s="164"/>
+      <c r="AB29" s="164"/>
+      <c r="AC29" s="164"/>
+      <c r="AD29" s="164"/>
+      <c r="AE29" s="164"/>
+      <c r="AF29" s="164"/>
+      <c r="AG29" s="164"/>
+      <c r="AH29" s="164"/>
+      <c r="AI29" s="164"/>
+      <c r="AJ29" s="164"/>
+      <c r="AK29" s="164"/>
+      <c r="AL29" s="164"/>
+      <c r="AM29" s="164"/>
+      <c r="AN29" s="164"/>
+      <c r="AO29" s="164"/>
+      <c r="AP29" s="164"/>
+      <c r="AQ29" s="164"/>
+      <c r="AR29" s="164"/>
+      <c r="AS29" s="164"/>
+      <c r="AT29" s="164"/>
+      <c r="AU29" s="164"/>
+      <c r="AV29" s="164"/>
+      <c r="AW29" s="164"/>
+      <c r="AX29" s="164"/>
+      <c r="AY29" s="164"/>
+      <c r="AZ29" s="165"/>
       <c r="BA29" s="25"/>
     </row>
-    <row r="30" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C30" s="24"/>
       <c r="BA30" s="25"/>
     </row>
-    <row r="31" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C31" s="24"/>
       <c r="BA31" s="25"/>
     </row>
-    <row r="32" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:53" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="C32" s="24"/>
       <c r="BA32" s="25"/>
     </row>
-    <row r="33" spans="1:56" s="15" customFormat="1" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:56" s="15" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C33" s="26"/>
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
@@ -4626,14 +4596,14 @@
       <c r="AZ33" s="27"/>
       <c r="BA33" s="28"/>
     </row>
-    <row r="34" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:56" s="15" customFormat="1" ht="2.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:56" s="15" customFormat="1" ht="2.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:56" s="15" customFormat="1" ht="2.85" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:56" s="15" customFormat="1" ht="2.85" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="155" t="s">
         <v>34</v>
       </c>
@@ -4713,7 +4683,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="61"/>
       <c r="B42" s="61"/>
       <c r="C42" s="61"/>
@@ -4773,7 +4743,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="61"/>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
@@ -4833,7 +4803,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="143" t="s">
         <v>74</v>
       </c>
@@ -4901,7 +4871,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="127" t="s">
         <v>84</v>
       </c>
@@ -4965,7 +4935,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="127" t="s">
         <v>77</v>
       </c>
@@ -5029,7 +4999,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="127" t="s">
         <v>42</v>
       </c>
@@ -5095,7 +5065,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="125" t="s">
         <v>82</v>
       </c>
@@ -5163,7 +5133,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="136"/>
       <c r="B49" s="137"/>
       <c r="C49" s="137"/>
@@ -5225,7 +5195,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="62" t="s">
         <v>54</v>
       </c>
@@ -5271,15 +5241,15 @@
       <c r="AG50" s="62"/>
       <c r="AH50" s="62"/>
       <c r="AI50" s="62"/>
-      <c r="AJ50" s="62" t="s">
+      <c r="AJ50" s="186" t="s">
         <v>57</v>
       </c>
-      <c r="AK50" s="62"/>
-      <c r="AL50" s="62"/>
-      <c r="AM50" s="62"/>
-      <c r="AN50" s="62"/>
-      <c r="AO50" s="62"/>
-      <c r="AP50" s="62"/>
+      <c r="AK50" s="186"/>
+      <c r="AL50" s="186"/>
+      <c r="AM50" s="186"/>
+      <c r="AN50" s="186"/>
+      <c r="AO50" s="186"/>
+      <c r="AP50" s="186"/>
       <c r="AQ50" s="127" t="s">
         <v>81</v>
       </c>
@@ -5299,7 +5269,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="62"/>
       <c r="B51" s="62"/>
       <c r="C51" s="62"/>
@@ -5335,13 +5305,13 @@
       <c r="AG51" s="62"/>
       <c r="AH51" s="62"/>
       <c r="AI51" s="62"/>
-      <c r="AJ51" s="62"/>
-      <c r="AK51" s="62"/>
-      <c r="AL51" s="62"/>
-      <c r="AM51" s="62"/>
-      <c r="AN51" s="62"/>
-      <c r="AO51" s="62"/>
-      <c r="AP51" s="62"/>
+      <c r="AJ51" s="186"/>
+      <c r="AK51" s="186"/>
+      <c r="AL51" s="186"/>
+      <c r="AM51" s="186"/>
+      <c r="AN51" s="186"/>
+      <c r="AO51" s="186"/>
+      <c r="AP51" s="186"/>
       <c r="AQ51" s="142" t="s">
         <v>80</v>
       </c>
@@ -5361,7 +5331,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="62"/>
       <c r="B52" s="62"/>
       <c r="C52" s="62"/>
@@ -5397,13 +5367,13 @@
       <c r="AG52" s="62"/>
       <c r="AH52" s="62"/>
       <c r="AI52" s="62"/>
-      <c r="AJ52" s="62"/>
-      <c r="AK52" s="62"/>
-      <c r="AL52" s="62"/>
-      <c r="AM52" s="62"/>
-      <c r="AN52" s="62"/>
-      <c r="AO52" s="62"/>
-      <c r="AP52" s="62"/>
+      <c r="AJ52" s="186"/>
+      <c r="AK52" s="186"/>
+      <c r="AL52" s="186"/>
+      <c r="AM52" s="186"/>
+      <c r="AN52" s="186"/>
+      <c r="AO52" s="186"/>
+      <c r="AP52" s="186"/>
       <c r="AQ52" s="133" t="s">
         <v>62</v>
       </c>
@@ -5423,7 +5393,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="62" t="s">
         <v>55</v>
       </c>
@@ -5461,13 +5431,13 @@
       <c r="AG53" s="62"/>
       <c r="AH53" s="62"/>
       <c r="AI53" s="62"/>
-      <c r="AJ53" s="62"/>
-      <c r="AK53" s="62"/>
-      <c r="AL53" s="62"/>
-      <c r="AM53" s="62"/>
-      <c r="AN53" s="62"/>
-      <c r="AO53" s="62"/>
-      <c r="AP53" s="62"/>
+      <c r="AJ53" s="186"/>
+      <c r="AK53" s="186"/>
+      <c r="AL53" s="186"/>
+      <c r="AM53" s="186"/>
+      <c r="AN53" s="186"/>
+      <c r="AO53" s="186"/>
+      <c r="AP53" s="186"/>
       <c r="AQ53" s="133" t="s">
         <v>61</v>
       </c>
@@ -5487,7 +5457,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="62"/>
       <c r="B54" s="62"/>
       <c r="C54" s="62"/>
@@ -5523,13 +5493,13 @@
       <c r="AG54" s="62"/>
       <c r="AH54" s="62"/>
       <c r="AI54" s="62"/>
-      <c r="AJ54" s="62"/>
-      <c r="AK54" s="62"/>
-      <c r="AL54" s="62"/>
-      <c r="AM54" s="62"/>
-      <c r="AN54" s="62"/>
-      <c r="AO54" s="62"/>
-      <c r="AP54" s="62"/>
+      <c r="AJ54" s="186"/>
+      <c r="AK54" s="186"/>
+      <c r="AL54" s="186"/>
+      <c r="AM54" s="186"/>
+      <c r="AN54" s="186"/>
+      <c r="AO54" s="186"/>
+      <c r="AP54" s="186"/>
       <c r="AQ54" s="133" t="s">
         <v>60</v>
       </c>
@@ -5549,7 +5519,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:56" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="62"/>
       <c r="B55" s="62"/>
       <c r="C55" s="62"/>
@@ -5587,13 +5557,13 @@
       <c r="AG55" s="62"/>
       <c r="AH55" s="62"/>
       <c r="AI55" s="62"/>
-      <c r="AJ55" s="62"/>
-      <c r="AK55" s="62"/>
-      <c r="AL55" s="62"/>
-      <c r="AM55" s="62"/>
-      <c r="AN55" s="62"/>
-      <c r="AO55" s="62"/>
-      <c r="AP55" s="62"/>
+      <c r="AJ55" s="186"/>
+      <c r="AK55" s="186"/>
+      <c r="AL55" s="186"/>
+      <c r="AM55" s="186"/>
+      <c r="AN55" s="186"/>
+      <c r="AO55" s="186"/>
+      <c r="AP55" s="186"/>
       <c r="AQ55" s="125" t="s">
         <v>59</v>
       </c>
@@ -5613,257 +5583,257 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="65" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="66" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="67" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="68" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="69" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="70" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="71" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="72" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="73" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="74" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="75" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="76" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="77" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="78" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="79" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="80" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="81" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="82" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="83" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="84" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="85" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="86" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="87" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="88" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="89" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="90" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="91" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="92" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="93" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="94" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="95" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="96" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="97" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="98" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="99" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="100" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="101" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="102" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="103" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="104" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="105" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="106" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="107" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="108" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="109" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="110" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="111" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="112" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="113" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="114" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="115" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="116" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="117" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="118" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="119" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="120" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="121" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="122" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="123" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="124" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="125" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="126" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="127" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="128" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="129" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="130" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="131" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="132" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="133" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="134" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="135" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="136" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="137" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="138" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="139" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="140" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="141" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="142" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="143" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="144" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="145" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="146" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="147" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="148" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="149" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="150" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="151" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="152" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="153" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="154" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="155" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="156" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="157" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="158" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="159" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="160" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="161" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="162" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="163" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="164" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="165" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="166" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="167" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="168" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="169" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="170" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="171" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="172" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="173" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="174" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="175" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="176" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="177" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="178" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="179" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="180" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="181" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="182" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="183" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="184" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="185" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="186" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="187" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="188" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="189" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="190" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="191" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="192" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="193" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="194" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="195" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="196" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="197" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="198" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="199" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="200" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="201" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="202" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="203" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="204" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="205" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="206" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="207" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="208" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="209" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="210" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="211" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="212" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="213" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="214" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="215" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="216" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="217" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="218" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="219" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="220" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="221" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="222" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="223" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="224" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="225" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="226" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="227" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="228" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="229" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="230" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="231" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="232" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="233" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="234" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="235" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="236" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="237" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="238" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="239" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="240" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="241" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="242" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="243" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="244" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="245" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="246" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="247" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="248" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="249" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="250" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="251" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="252" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="253" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="254" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="255" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="256" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="257" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="258" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="259" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="260" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="261" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="262" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="263" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="264" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="265" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="266" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="267" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="268" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="269" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="270" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="271" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="272" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="273" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="274" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="275" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="276" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="277" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="278" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="279" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="280" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="281" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="282" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="283" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="284" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="285" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="286" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="287" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="288" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="289" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="290" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="291" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="292" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="293" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="294" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="295" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="296" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="297" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="298" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="299" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="300" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="301" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="302" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="303" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="304" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="305" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
-    <row r="306" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:56" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="65" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="66" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="67" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="68" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="69" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="70" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="71" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="72" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="73" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="74" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="75" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="76" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="77" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="78" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="79" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="80" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="81" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="82" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="83" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="84" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="85" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="86" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="87" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="88" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="89" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="90" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="91" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="92" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="93" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="94" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="95" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="96" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="97" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="98" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="99" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="100" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="101" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="102" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="103" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="104" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="105" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="106" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="107" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="108" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="109" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="110" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="111" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="112" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="113" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="114" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="115" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="116" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="117" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="118" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="119" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="120" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="121" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="122" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="123" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="124" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="125" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="126" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="127" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="128" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="129" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="130" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="131" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="132" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="133" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="134" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="135" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="136" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="137" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="138" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="139" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="140" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="141" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="142" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="143" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="144" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="145" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="146" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="147" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="148" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="149" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="150" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="151" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="152" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="153" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="154" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="155" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="156" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="157" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="158" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="159" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="160" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="161" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="162" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="163" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="164" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="165" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="166" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="167" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="168" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="169" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="170" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="171" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="172" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="173" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="174" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="175" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="176" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="177" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="178" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="179" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="180" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="181" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="182" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="183" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="184" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="185" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="186" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="187" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="188" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="189" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="190" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="191" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="192" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="193" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="194" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="195" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="196" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="197" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="198" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="199" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="200" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="201" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="202" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="203" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="204" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="205" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="206" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="207" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="208" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="209" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="210" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="211" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="212" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="213" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="214" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="215" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="216" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="217" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="218" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="219" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="220" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="221" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="222" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="223" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="224" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="225" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="226" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="227" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="228" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="229" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="230" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="231" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="232" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="233" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="234" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="235" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="236" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="237" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="238" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="239" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="240" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="241" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="242" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="243" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="244" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="245" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="246" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="247" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="248" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="249" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="250" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="251" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="252" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="253" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="254" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="255" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="256" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="257" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="258" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="259" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="260" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="261" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="262" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="263" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="264" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="265" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="266" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="267" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="268" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="269" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="270" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="271" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="272" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="273" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="274" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="275" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="276" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="277" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="278" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="279" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="280" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="281" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="282" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="283" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="284" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="285" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="286" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="287" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="288" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="289" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="290" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="291" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="292" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="293" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="294" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="295" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="296" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="297" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="298" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="299" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="300" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="301" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="302" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="303" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="304" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="305" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
+    <row r="306" s="15" customFormat="1" ht="12" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="94">
     <mergeCell ref="P21:Z21"/>
@@ -5975,18 +5945,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" customWidth="1"/>
-    <col min="16" max="17" width="9.1796875" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="26" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="110" t="s">
         <v>0</v>
       </c>
@@ -5996,11 +5966,11 @@
       <c r="F2" s="114"/>
       <c r="G2" s="114"/>
       <c r="H2" s="114"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="163"/>
-      <c r="K2" s="158"/>
-    </row>
-    <row r="3" spans="2:14" ht="21" x14ac:dyDescent="0.5">
+      <c r="I2" s="172"/>
+      <c r="J2" s="172"/>
+      <c r="K2" s="167"/>
+    </row>
+    <row r="3" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="116" t="s">
         <v>15</v>
       </c>
@@ -6010,14 +5980,14 @@
       <c r="F3" s="120"/>
       <c r="G3" s="120"/>
       <c r="H3" s="120"/>
-      <c r="I3" s="163"/>
-      <c r="J3" s="163"/>
-      <c r="K3" s="158"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="I3" s="172"/>
+      <c r="J3" s="172"/>
+      <c r="K3" s="167"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G4" s="4"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="95" t="s">
         <v>16</v>
       </c>
@@ -6027,7 +5997,7 @@
       <c r="F6" s="108"/>
       <c r="G6" s="108"/>
       <c r="H6" s="108"/>
-      <c r="I6" s="158"/>
+      <c r="I6" s="167"/>
       <c r="K6" s="177" t="s">
         <v>85</v>
       </c>
@@ -6035,7 +6005,7 @@
       <c r="M6" s="178"/>
       <c r="N6" s="179"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="95" t="s">
         <v>17</v>
       </c>
@@ -6045,13 +6015,13 @@
       <c r="F7" s="108"/>
       <c r="G7" s="108"/>
       <c r="H7" s="108"/>
-      <c r="I7" s="158"/>
+      <c r="I7" s="167"/>
       <c r="K7" s="180"/>
       <c r="L7" s="181"/>
       <c r="M7" s="181"/>
       <c r="N7" s="182"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="95" t="s">
         <v>18</v>
       </c>
@@ -6061,13 +6031,13 @@
       <c r="F8" s="108"/>
       <c r="G8" s="108"/>
       <c r="H8" s="108"/>
-      <c r="I8" s="158"/>
+      <c r="I8" s="167"/>
       <c r="K8" s="180"/>
       <c r="L8" s="181"/>
       <c r="M8" s="181"/>
       <c r="N8" s="182"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="95" t="s">
         <v>19</v>
       </c>
@@ -6077,13 +6047,13 @@
       <c r="F9" s="108"/>
       <c r="G9" s="108"/>
       <c r="H9" s="108"/>
-      <c r="I9" s="158"/>
+      <c r="I9" s="167"/>
       <c r="K9" s="180"/>
       <c r="L9" s="181"/>
       <c r="M9" s="181"/>
       <c r="N9" s="182"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="95" t="s">
         <v>20</v>
       </c>
@@ -6093,13 +6063,13 @@
       <c r="F10" s="99"/>
       <c r="G10" s="99"/>
       <c r="H10" s="99"/>
-      <c r="I10" s="158"/>
+      <c r="I10" s="167"/>
       <c r="K10" s="183"/>
       <c r="L10" s="184"/>
       <c r="M10" s="184"/>
       <c r="N10" s="185"/>
     </row>
-    <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="44"/>
@@ -6108,7 +6078,7 @@
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
     </row>
-    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B14" s="45"/>
       <c r="C14" s="46"/>
       <c r="D14" s="46"/>
@@ -6123,84 +6093,84 @@
       <c r="M14" s="42"/>
       <c r="N14" s="43"/>
     </row>
-    <row r="15" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="164" t="s">
+    <row r="15" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="173" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="165"/>
-      <c r="E15" s="165"/>
-      <c r="F15" s="165"/>
-      <c r="G15" s="167"/>
-      <c r="I15" s="164" t="s">
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="174"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="176"/>
+      <c r="I15" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="J15" s="165"/>
-      <c r="K15" s="165"/>
-      <c r="L15" s="165"/>
-      <c r="M15" s="165"/>
-      <c r="N15" s="166"/>
-    </row>
-    <row r="16" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="164"/>
-      <c r="C16" s="165"/>
-      <c r="D16" s="165"/>
-      <c r="E16" s="165"/>
-      <c r="F16" s="165"/>
-      <c r="G16" s="167"/>
+      <c r="J15" s="174"/>
+      <c r="K15" s="174"/>
+      <c r="L15" s="174"/>
+      <c r="M15" s="174"/>
+      <c r="N15" s="175"/>
+    </row>
+    <row r="16" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="173"/>
+      <c r="C16" s="174"/>
+      <c r="D16" s="174"/>
+      <c r="E16" s="174"/>
+      <c r="F16" s="174"/>
+      <c r="G16" s="176"/>
       <c r="H16" s="30"/>
-      <c r="I16" s="164"/>
-      <c r="J16" s="165"/>
-      <c r="K16" s="165"/>
-      <c r="L16" s="165"/>
-      <c r="M16" s="165"/>
-      <c r="N16" s="166"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="I16" s="173"/>
+      <c r="J16" s="174"/>
+      <c r="K16" s="174"/>
+      <c r="L16" s="174"/>
+      <c r="M16" s="174"/>
+      <c r="N16" s="175"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
       <c r="G17" s="34"/>
       <c r="I17" s="33"/>
       <c r="N17" s="34"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="33"/>
       <c r="G18" s="34"/>
       <c r="I18" s="33"/>
       <c r="N18" s="34"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="33"/>
-      <c r="C19" s="159" t="s">
+      <c r="C19" s="168" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="160"/>
-      <c r="G19" s="161"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="168"/>
+      <c r="F19" s="169"/>
+      <c r="G19" s="170"/>
       <c r="I19" s="33"/>
-      <c r="J19" s="162" t="s">
+      <c r="J19" s="171" t="s">
         <v>71</v>
       </c>
-      <c r="K19" s="162"/>
-      <c r="L19" s="162"/>
-      <c r="M19" s="160"/>
-      <c r="N19" s="161"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="K19" s="171"/>
+      <c r="L19" s="171"/>
+      <c r="M19" s="169"/>
+      <c r="N19" s="170"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="33"/>
-      <c r="C20" s="159"/>
-      <c r="D20" s="159"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="160"/>
-      <c r="G20" s="161"/>
+      <c r="C20" s="168"/>
+      <c r="D20" s="168"/>
+      <c r="E20" s="168"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="170"/>
       <c r="I20" s="33"/>
-      <c r="J20" s="162"/>
-      <c r="K20" s="162"/>
-      <c r="L20" s="162"/>
-      <c r="M20" s="160"/>
-      <c r="N20" s="161"/>
-    </row>
-    <row r="21" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="J20" s="171"/>
+      <c r="K20" s="171"/>
+      <c r="L20" s="171"/>
+      <c r="M20" s="169"/>
+      <c r="N20" s="170"/>
+    </row>
+    <row r="21" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="35"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -6211,46 +6181,46 @@
       <c r="I21" s="33"/>
       <c r="N21" s="34"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
       <c r="G22" s="34"/>
       <c r="I22" s="33"/>
       <c r="N22" s="34"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
-      <c r="C23" s="159" t="s">
+      <c r="C23" s="168" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="159"/>
-      <c r="E23" s="159"/>
-      <c r="F23" s="160"/>
-      <c r="G23" s="161"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="169"/>
+      <c r="G23" s="170"/>
       <c r="I23" s="33"/>
-      <c r="J23" s="162" t="s">
+      <c r="J23" s="171" t="s">
         <v>73</v>
       </c>
-      <c r="K23" s="162"/>
-      <c r="L23" s="162"/>
-      <c r="M23" s="160"/>
-      <c r="N23" s="161"/>
-    </row>
-    <row r="24" spans="2:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="K23" s="171"/>
+      <c r="L23" s="171"/>
+      <c r="M23" s="169"/>
+      <c r="N23" s="170"/>
+    </row>
+    <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="35"/>
-      <c r="C24" s="159"/>
-      <c r="D24" s="159"/>
-      <c r="E24" s="159"/>
-      <c r="F24" s="160"/>
-      <c r="G24" s="161"/>
+      <c r="C24" s="168"/>
+      <c r="D24" s="168"/>
+      <c r="E24" s="168"/>
+      <c r="F24" s="169"/>
+      <c r="G24" s="170"/>
       <c r="H24" s="30"/>
       <c r="I24" s="33"/>
-      <c r="J24" s="162"/>
-      <c r="K24" s="162"/>
-      <c r="L24" s="162"/>
-      <c r="M24" s="160"/>
-      <c r="N24" s="161"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="J24" s="171"/>
+      <c r="K24" s="171"/>
+      <c r="L24" s="171"/>
+      <c r="M24" s="169"/>
+      <c r="N24" s="170"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="37"/>
       <c r="C25" s="32"/>
       <c r="D25" s="32"/>
@@ -6263,7 +6233,7 @@
       <c r="M25" s="31"/>
       <c r="N25" s="49"/>
     </row>
-    <row r="26" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="38"/>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
@@ -6277,24 +6247,24 @@
       <c r="M26" s="39"/>
       <c r="N26" s="40"/>
     </row>
-    <row r="27" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="2:15" ht="31" x14ac:dyDescent="0.7">
-      <c r="B29" s="157" t="s">
+    <row r="27" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:15" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B29" s="166" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="157"/>
-      <c r="D29" s="157"/>
-      <c r="E29" s="157"/>
-      <c r="F29" s="157"/>
-      <c r="G29" s="157"/>
-      <c r="H29" s="157"/>
-      <c r="I29" s="157"/>
-      <c r="J29" s="157"/>
-      <c r="K29" s="157"/>
-      <c r="L29" s="157"/>
-      <c r="M29" s="157"/>
-      <c r="N29" s="157"/>
-      <c r="O29" s="157"/>
+      <c r="C29" s="166"/>
+      <c r="D29" s="166"/>
+      <c r="E29" s="166"/>
+      <c r="F29" s="166"/>
+      <c r="G29" s="166"/>
+      <c r="H29" s="166"/>
+      <c r="I29" s="166"/>
+      <c r="J29" s="166"/>
+      <c r="K29" s="166"/>
+      <c r="L29" s="166"/>
+      <c r="M29" s="166"/>
+      <c r="N29" s="166"/>
+      <c r="O29" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="26">

</xml_diff>